<commit_message>
Solved synchronous execution for Email generation process
</commit_message>
<xml_diff>
--- a/policy failure.xlsx
+++ b/policy failure.xlsx
@@ -427,6 +427,64 @@
     <row>
       <c t="inlineStr" s="">
         <is>
+          <t>FCM1131972</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>CAP825</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>V2P-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Exception class = org.springframework.web.client.HttpClientErrorException, with id = V20180508-142718.CAP825.FCM1131972-2-3@20180508-142718.580, statusCode = 400, responseBody = &lt;error&gt;
+&lt;code&gt;400&lt;/code&gt;
+&lt;message&gt;Hibernate operation: Could not execute JDBC batch update; SQL [insert into LINKS (LINK_FROM_PRODUCT_CODE, LINK_FROM_POLICY_NUMBER, LINK_FROM_HISTORY_NUMBER, LINK_TO_PRODUCT_CODE, LINK_TO_POLICY_NUMBER, LINK_TO_HISTORY_NUMBER, LINK_TYPE) values (?, ?, ?, ?, ?, ?, ?)]; ORA-00001: unique constraint (OPS$TUPPDBA.LINK_PK_PRIM) violated ; nested exception is java.sql.BatchUpdateException: ORA-00001: unique constraint (OPS$TUPPDBA.LINK_PK_PRIM) violated&lt;/message&gt;
+&lt;/error&gt;
+</t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>FCM1133262</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>VANV100</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>V2P-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>500</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Exception class = org.springframework.web.client.HttpServerErrorException, with id = V20180510-125401.VANV100.FCM1133262-1-5@20180510-125401.834, statusCode = 500, responseBody = &lt;error&gt;
+&lt;code&gt;500&lt;/code&gt;
+&lt;message&gt;NullPointerException&lt;/message&gt;
+&lt;/error&gt;
+</t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
           <t>TMI3231706</t>
         </is>
       </c>
@@ -1146,6 +1204,3487 @@
       <c t="inlineStr" s="">
         <is>
           <t>!sales.sys.error.policy.amend.version.database.mismatch!. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3233174</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA004</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3233174-2, however cannot find the corresponding source policy TMI3233174-1.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3275543</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA021</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>sales.app.error.cannot.renew.policy.newer.version.exists: Conflict in saving policy TMI3275543-1-0, it has a linked source policy TMI3231053-1-1, which has newer versions: [TMI3275538-1-0]. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3184497</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA021</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3184497-3, however cannot find the corresponding source policy TMI3184497-2.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3268834</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA024</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>sales.app.error.cannot.renew.policy.newer.version.exists: Conflict in saving policy TMI3268834-1-0, it has a linked source policy TMI2730595-8-0, which has newer versions: [TMI3218620-1-0]. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI2998157</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA024</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI2998157-6, however cannot find the corresponding source policy TMI2998157-5.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3231945</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA025</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>sales.app.error.cannot.renew.policy.newer.version.exists: Conflict in saving policy TMI3231945-2-0, it has a linked source policy TMI3111393-1-0, which has newer versions: [TMI3231945-1-0]. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3182979</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA025</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3182979-3, however cannot find the corresponding source policy TMI3182979-2.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3233484</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA030</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>sales.app.error.cannot.renew.policy.newer.version.exists: Conflict in saving policy TMI3233484-1-0, it has a linked source policy TMI2803459-6-0, which has newer versions: [TMI3182542-1-0]. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3068590</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA030</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3068590-5, however cannot find the corresponding source policy TMI3068590-4.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3233485</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA030</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3233485-2, however cannot find the corresponding source policy TMI3233485-1.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3281857</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA030</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>sales.app.error.cannot.renew.policy.newer.version.exists: Conflict in saving policy TMI3281857-1-0, it has a linked source policy TMI3142092-1-0, which has newer versions: [TMI3205119-1-0]. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3281912</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA030</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>sales.app.error.cannot.renew.policy.newer.version.exists: Conflict in saving policy TMI3281912-1-0, it has a linked source policy TMI3216058-1-0, which has newer versions: [TMI3281910-1-0]. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3281934</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA030</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>sales.app.error.cannot.renew.policy.newer.version.exists: Conflict in saving policy TMI3281934-1-0, it has a linked source policy TMI2989618-5-0, which has newer versions: [TMI3281933-1-0]. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3281932</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA030</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>sales.app.error.cannot.renew.policy.newer.version.exists: Conflict in saving policy TMI3281932-1-0, it has a linked source policy TMI2989618-5-0, which has newer versions: [TMI3281933-1-0]. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3281936</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA030</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>sales.app.error.cannot.renew.policy.newer.version.exists: Conflict in saving policy TMI3281936-1-0, it has a linked source policy TMI2989618-5-0, which has newer versions: [TMI3281933-1-0]. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3282012</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA030</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>sales.app.error.cannot.renew.policy.newer.version.exists: Conflict in saving policy TMI3282012-1-0, it has a linked source policy TMI3172929-1-0, which has newer versions: [TMI3231900-1-0]. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3235429</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA062</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3235429-2, however cannot find the corresponding source policy TMI3235429-1.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3278152</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA063</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>sales.app.error.cannot.renew.policy.newer.version.exists: Conflict in saving policy TMI3278152-1-0, it has a linked source policy TMI3128457-3-1, which has newer versions: [TMI3278149-1-0]. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3278151</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA063</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>sales.app.error.cannot.renew.policy.newer.version.exists: Conflict in saving policy TMI3278151-1-0, it has a linked source policy TMI3128457-3-1, which has newer versions: [TMI3278149-1-0]. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3241472</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA075</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3241472-1, however cannot find the corresponding source policy TMI2756038-9.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3274150</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA075</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>sales.app.error.cannot.renew.policy.newer.version.exists: Conflict in saving policy TMI3274150-1-0, it has a linked source policy TMI3221381-1-1, which has newer versions: [TMI3274145-1-0]. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TSI2987444</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA075</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>could not apply rider: code=PM-SPRT-17 to person:PHX-PERSON-3017784342613120-1. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TSI2987506</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA075</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>could not apply rider: code=PM-SPRT-17 to person:PHX-PERSON-3019956856004915-1. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3282011</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA075</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3282011-1, however cannot find the corresponding source policy TMI3239431-1.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3184638</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA086</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3184638-3, however cannot find the corresponding source policy TMI3184638-2.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3184639</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA086</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3184639-3, however cannot find the corresponding source policy TMI3184639-2.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI2866843</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA090</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI2866843-8, however cannot find the corresponding source policy TMI2866843-7.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3067793</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA097</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3067793-5, however cannot find the corresponding source policy TMI3067793-4.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>FCS1720721</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>571848</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>!sales.app.error.policy.save.failed!. Sending alert email failed: exception = org.springframework.web.client.HttpServerErrorException, statusCode = 500, responseBody = {"status":"error","code":-1,"name":"ValidationError","message":"You must specify a key value"}</t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>SCN537667</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>LAS23840</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>!sales.sys.error.policy.amend.version.database.mismatch!. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3247624</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA030</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>sales.app.error.cannot.renew.policy.newer.version.exists: Conflict in saving policy TMI3247624-1-0, it has a linked source policy TMI3046744-4-0, which has newer versions: [TMI3046744-5-0]. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>FGM1177432</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>COU513</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + !sales.drl.error.rule.rider.selection.not.applied.all.family.plans.summary!. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>FGM1155203</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>PAG340</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>sales.app.error.cannot.renew.policy.newer.version.exists: Conflict in saving policy FGM1155203-2-0, it has a linked source policy FGM1155203-1-0, which has newer versions: [QOT9243815]. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>FCM1131428</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TOS307</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>sales.app.error.cannot.renew.policy.newer.version.exists: Conflict in saving policy FCM1131428-2-0, it has a linked source policy FCM1131428-1-0, which has newer versions: [QOT9243327]. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>FCM1131428</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TOS307</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>sales.app.error.cannot.renew.policy.newer.version.exists: Conflict in saving policy FCM1131428-2-0, it has a linked source policy FCM1131428-1-0, which has newer versions: [QOT9243327]. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>FCM1131428</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TOS307</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>sales.app.error.cannot.renew.policy.newer.version.exists: Conflict in saving policy FCM1131428-2-0, it has a linked source policy FCM1131428-1-0, which has newer versions: [QOT9243327]. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>FCM1166292</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BAR518</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>sales.app.error.cannot.renew.policy.newer.version.exists: Conflict in saving policy FCM1166292-0-0, it has a linked source policy FGM1153721-1-0, which has newer versions: [QOT9243786]. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>FCM1166292</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BAR518</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>sales.app.error.cannot.renew.policy.newer.version.exists: Conflict in saving policy FCM1166292-0-0, it has a linked source policy FGM1153721-1-0, which has newer versions: [QOT9243786]. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>FCM1166292</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BAR518</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>sales.app.error.cannot.renew.policy.newer.version.exists: Conflict in saving policy FCM1166292-0-0, it has a linked source policy FGM1153721-1-0, which has newer versions: [QOT9243786]. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>FCM1166292</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BAR518</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>sales.app.error.cannot.renew.policy.newer.version.exists: Conflict in saving policy FCM1166292-0-0, it has a linked source policy FGM1153721-1-0, which has newer versions: [QOT9243786]. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3233572</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA004</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>sales.app.error.cannot.renew.policy.newer.version.exists: Conflict in saving policy TMI3233572-2-0, it has a linked source policy TMI2795963-6-0, which has newer versions: [TMI3233572-1-0]. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3232222</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA024</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3232222-2, however cannot find the corresponding source policy TMI3232222-1.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3180625</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA024</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3180625-3, however cannot find the corresponding source policy TMI3180625-2.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3226841</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA025</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3226841-2, however cannot find the corresponding source policy TMI3226841-1.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3227364</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA030</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3227364-2, however cannot find the corresponding source policy TMI3227364-1.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3279675</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA030</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3279675-1, however cannot find the corresponding source policy TMI3254972-1.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3231825</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA030</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>sales.app.error.cannot.renew.policy.newer.version.exists: Conflict in saving policy TMI3231825-2-0, it has a linked source policy TMI3058659-2-0, which has newer versions: [TMI3177717-1-0]. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3281804</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA030</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>sales.app.error.cannot.renew.policy.newer.version.exists: Conflict in saving policy TMI3281804-2-0, it has a linked source policy TMI3231154-1-1, which has newer versions: [TMI3281804-1-0]. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI2921038</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA030</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI2921038-7, however cannot find the corresponding source policy TMI2921038-6.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3185225</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA030</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3185225-3, however cannot find the corresponding source policy TMI3185225-2.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3235810</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA030</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3235810-2, however cannot find the corresponding source policy TMI3235810-1.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3237482</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA030</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3237482-2, however cannot find the corresponding source policy TMI3237482-1.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3282027</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA030</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3282027-1, however cannot find the corresponding source policy TMI3236554-1.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3282077</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA030</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>sales.app.error.cannot.renew.policy.newer.version.exists: Conflict in saving policy TMI3282077-1-0, it has a linked source policy TMI2978044-3-0, which has newer versions: [TMI3172196-1-0, TMI3172197-1-0]. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3234916</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA031</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3234916-2, however cannot find the corresponding source policy TMI3234916-1.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3232830</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA041</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>sales.app.error.cannot.renew.policy.newer.version.exists: Conflict in saving policy TMI3232830-2-0, it has a linked source policy TMI2921880-4-0, which has newer versions: [TMI3232830-1-0]. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3069094</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA043</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3069094-5, however cannot find the corresponding source policy TMI3069094-4.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3069092</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA043</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3069092-5, however cannot find the corresponding source policy TMI3069092-4.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3236004</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA043</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3236004-2, however cannot find the corresponding source policy TMI3236004-1.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TSI2985833</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA062</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>product:TSI unable to transform questionnaire. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3182119</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA062</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3182119-2, however cannot find the corresponding source policy TMI3182119-1.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TSI2986900</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA075</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>could not apply rider: code=PM-SPRT-17 to person:PHX-PERSON-3101937885813847-1. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI2927634</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA075</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI2927634-7, however cannot find the corresponding source policy TMI2927634-6.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TSI2988039</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA075</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Effective Date must be set after or same as Application Date. Adjust the Effective and/or Application Date.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3282104</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA081</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3282104-1, however cannot find the corresponding source policy TMI3230854-1.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3139165</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA082</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3139165-4, however cannot find the corresponding source policy TMI3139165-3.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3139167</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA082</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3139167-4, however cannot find the corresponding source policy TMI3139167-3.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3282039</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA085</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>sales.app.error.cannot.renew.policy.newer.version.exists: Conflict in saving policy TMI3282039-1-0, it has a linked source policy TMI3121046-1-0, which has newer versions: [TMI3195640-1-0]. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3228639</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA025</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>sales.app.error.cannot.renew.policy.newer.version.exists: Conflict in saving policy TMI3228639-1-0, it has a linked source policy TMI3063221-3-0, which has newer versions: [TMI3063221-4-0]. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>FCM1166292</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BAR518</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>sales.app.error.cannot.renew.policy.newer.version.exists: Conflict in saving policy FCM1166292-0-0, it has a linked source policy FGM1153721-1-0, which has newer versions: [QOT9243786]. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>FCM1166292</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BAR518</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>sales.app.error.cannot.renew.policy.newer.version.exists: Conflict in saving policy FCM1166292-0-0, it has a linked source policy FGM1153721-1-0, which has newer versions: [QOT9243786]. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>FCS1726892</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>MAWSA</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>POLICY_PRIMARY_ADDRESS_REQUIRED. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>FCS1726893</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>MAWSA</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>POLICY_PRIMARY_ADDRESS_REQUIRED. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3277292</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA024</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>sales.app.error.cannot.renew.policy.newer.version.exists: Conflict in saving policy TMI3277292-1-0, it has a linked source policy TMI2640032-11-1, which has newer versions: [TMI3277291-1-0]. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3257318</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA030</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>sales.app.error.cannot.renew.policy.newer.version.exists: Conflict in saving policy TMI3257318-1-0, it has a linked source policy TMI2829943-7-0, which has newer versions: [TMI3217755-1-0]. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3173596</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA030</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3173596-3, however cannot find the corresponding source policy TMI3210132-2.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3173595</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA030</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3173595-3, however cannot find the corresponding source policy TMI3210120-2.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI2696861</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA030</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI2696861-11, however cannot find the corresponding source policy TMI2696861-10.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI2802410</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA030</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>could not apply rider: code=PM-SPRT-11 to person:PHX-PERSON-3190045236674508-1. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI2989605</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA030</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI2989605-6, however cannot find the corresponding source policy TMI2989605-5.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3132833</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA030</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3132833-4, however cannot find the corresponding source policy TMI3132833-3.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3185531</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA030</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3185531-3, however cannot find the corresponding source policy TMI3185531-2.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3185532</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA030</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3185532-3, however cannot find the corresponding source policy TMI3185532-2.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3188948</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA030</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3188948-3, however cannot find the corresponding source policy TMI3188948-2.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3282204</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA030</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>sales.app.error.cannot.renew.policy.newer.version.exists: Conflict in saving policy TMI3282204-1-0, it has a linked source policy TMI3065438-4-1, which has newer versions: [TMI3282203-1-0]. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3282287</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA030</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3282287-1, however cannot find the corresponding source policy TMI3186196-2.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3237998</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA041</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3237998-2, however cannot find the corresponding source policy TMI3237998-1.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3282304</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA041</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3282304-1, however cannot find the corresponding source policy TMI3180131-2.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TSI2984984</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA042</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>product:TSI unable to transform questionnaire. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3063585</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA044</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3063585-5, however cannot find the corresponding source policy TMI3063585-4.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3232822</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA044</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>sales.app.error.cannot.renew.policy.newer.version.exists: Conflict in saving policy TMI3232822-2-0, it has a linked source policy TMI3210826-1-1, which has newer versions: [TMI3232822-1-0]. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI2931385</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA075</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI2931385-7, however cannot find the corresponding source policy TMI2931385-6.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3176595</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA075</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3176595-3, however cannot find the corresponding source policy TMI3176595-2.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3235211</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA075</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3235211-2, however cannot find the corresponding source policy TMI3235211-1.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3282315</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA075</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3282315-1, however cannot find the corresponding source policy TMI3235333-1.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TSI2989035</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA075</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>could not apply rider: code=PM-SPRT-11 to person:PHX-PERSON-3188447674034353-1. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3181907</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA085</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3181907-3, however cannot find the corresponding source policy TMI3181907-2.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3232265</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA087</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3232265-2, however cannot find the corresponding source policy TMI3232265-1.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3236021</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA097</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3236021-2, however cannot find the corresponding source policy TMI3236021-1.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3235308</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA097</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3235308-2, however cannot find the corresponding source policy TMI3235308-1.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>FCM1148234</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>WG1VAN</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>!sales.sys.error.policy.amend.version.database.mismatch!. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>FCS1721973</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>WG2HIR</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>!sales.sys.error.policy.amend.version.database.mismatch!. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>FGS1734666</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BTE525</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>!sales.app.error.policy.save.failed!. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>FCS4783170</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>MCB024</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>!sales.sys.error.policy.amend.version.database.mismatch!. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>FGM1139098</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>WHI850</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>sales.app.error.cannot.renew.policy.newer.version.exists: Conflict in saving policy FGM1139098-3-0, it has a linked source policy FGM1139098-2-0, which has newer versions: [QOT9244216]. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>VMD1072696</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>KAR188</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>504</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Phoenix2Venture ERROR: Exception class = org.springframework.web.client.HttpServerErrorException, with id = M20180510-202527.KAR188.VMD1072696-0, statusCode = 504, responseBody = &lt;html&gt;
+&lt;head&gt;&lt;title&gt;504 Gateway Time-out&lt;/title&gt;&lt;/head&gt;
+&lt;body bgcolor="white"&gt;
+&lt;center&gt;&lt;h1&gt;504 Gateway Time-out&lt;/h1&gt;&lt;/center&gt;
+&lt;/body&gt;
+&lt;/html&gt;
+. Sending alert email failed: exception = org.springframework.web.client.HttpServerErrorException, statusCode = 500, responseBody = {"status":"error","code":-1,"name":"ValidationError","message":"You must specify a key value"}</t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3237771</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA001</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3237771-2, however cannot find the corresponding source policy TMI3237771-1.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3282400</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA001</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>could not apply rider: code=PM-SPRT-17 to person:PHX-PERSON-3273948523345650-1. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3282487</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA004</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>sales.app.error.cannot.renew.policy.newer.version.exists: Conflict in saving policy TMI3282487-1-0, it has a linked source policy TMI3229802-1-1, which has newer versions: [TMI3282488-1-0]. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3282218</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA021</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3282218-1, however cannot find the corresponding source policy TMI3228639-1.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3184265</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA022</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3184265-3, however cannot find the corresponding source policy TMI3184265-2.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3184265</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA022</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3184265-3, however cannot find the corresponding source policy TMI3184265-2.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI2930814</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA024</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI2930814-7, however cannot find the corresponding source policy TMI2930814-6.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3241905</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA030</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>sales.app.error.cannot.renew.policy.newer.version.exists: Conflict in saving policy TMI3241905-1-0, it has a linked source policy TMI2940886-5-0, which has newer versions: [TMI2940886-6-0]. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3268767</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA030</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>sales.app.error.cannot.renew.policy.newer.version.exists: Conflict in saving policy TMI3268767-1-0, it has a linked source policy TMI3220952-1-0, which has newer versions: [TMI3251831-1-0]. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3128880</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA030</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>could not apply rider: code=PM-SPRT-11 to person:PHX-PERSON-3278525788362320-1. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3231356</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA030</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>sales.app.error.cannot.renew.policy.newer.version.exists: Conflict in saving policy TMI3231356-2-0, it has a linked source policy TMI3126262-2-0, which has newer versions: [TMI3231356-1-0]. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3235138</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA030</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3235138-2, however cannot find the corresponding source policy TMI3235138-1.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3235140</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA030</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3235140-2, however cannot find the corresponding source policy TMI3235140-1.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3236704</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA030</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3236704-2, however cannot find the corresponding source policy TMI3236704-1.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3175232</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA043</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3175232-3, however cannot find the corresponding source policy TMI3175232-2.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI2567813</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA061</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI2567813-13, however cannot find the corresponding source policy TMI2567813-12.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI2645514</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA061</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI2645514-12, however cannot find the corresponding source policy TMI2645514-11.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI2864183</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA061</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI2864183-8, however cannot find the corresponding source policy TMI2864183-7.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3232648</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA061</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>sales.app.error.cannot.renew.policy.newer.version.exists: Conflict in saving policy TMI3232648-2-0, it has a linked source policy TMI3147720-1-0, which has newer versions: [TMI3232648-1-0]. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3282384</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA065</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>sales.app.error.cannot.renew.policy.newer.version.exists: Conflict in saving policy TMI3282384-1-0, it has a linked source policy TMI3175836-1-0, which has newer versions: [TMI3229860-1-0]. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3282382</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA065</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>sales.app.error.cannot.renew.policy.newer.version.exists: Conflict in saving policy TMI3282382-1-0, it has a linked source policy TMI3175837-1-0, which has newer versions: [TMI3229861-1-0]. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3125031</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA075</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>could not apply rider: code=PM-SPRT-11 to person:PHX-PERSON-3274586972675981-1. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3281542</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA075</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>could not apply rider: code=PM-SPRT-17 to person:PHX-PERSON-3277729690585332-1. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3235316</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA075</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3235316-2, however cannot find the corresponding source policy TMI3235316-1.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3282494</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA075</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3282494-1, however cannot find the corresponding source policy TMI3241083-1.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3282357</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA083</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3282357-1, however cannot find the corresponding source policy TMI3025479-5.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3282362</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA083</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3282362-1, however cannot find the corresponding source policy TMI3025483-5.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3129679</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA084</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>could not apply rider: code=PM-SPRT-11 to person:PHX-PERSON-3277976540882060-1. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3240836</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA085</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3240836-2, however cannot find the corresponding source policy TMI3240836-1.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>TMI3067793</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>BCA097</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Error + Renew policy TMI3067793-5, however cannot find the corresponding source policy TMI3067793-4.. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>FCM1166371</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>528103</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>!sales.app.error.policy.save.failed!. </t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>VMD1074843</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>PRA218</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>!sales.sys.error.policy.amend.version.database.mismatch!. Sending alert email failed: exception = org.springframework.web.client.HttpServerErrorException, statusCode = 500, responseBody = {"status":"error","code":-1,"name":"ValidationError","message":"You must specify a key value"}</t>
+        </is>
+      </c>
+    </row>
+    <row>
+      <c t="inlineStr" s="">
+        <is>
+          <t>SGG130193</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>LEP480</t>
+        </is>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>P2V-POLICY-TRANSFER-STATUS</t>
+        </is>
+      </c>
+      <c s="">
+        <v>400</v>
+      </c>
+      <c t="inlineStr" s="">
+        <is>
+          <t>Product:SGG not found for partner:LEP480. </t>
         </is>
       </c>
     </row>

</xml_diff>